<commit_message>
Fix occurrence field in standard import
replaced `Encounter.occurrenceID` with `Encounter.sightingID`
</commit_message>
<xml_diff>
--- a/docs/assets/templates/WildbookStandardFormat.xlsx
+++ b/docs/assets/templates/WildbookStandardFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Desktop/New Bulk Import spreadsheet templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5566CBE9-C4F3-7A46-82BD-3625A7FB5FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135D5179-EC6B-4345-97A1-784F0FDAE50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35240" yWindow="1660" windowWidth="30240" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,9 +29,6 @@
     <t>MarkedIndividual.individualID</t>
   </si>
   <si>
-    <t>Encounter.occurrenceID</t>
-  </si>
-  <si>
     <t>Encounter.verbatimLocality</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Encounter.sightingRemarks</t>
+  </si>
+  <si>
+    <t>Encounter.sightingID</t>
   </si>
 </sst>
 </file>
@@ -443,79 +443,79 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -540,18 +540,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>